<commit_message>
Bulk of code for excel export and de-identification for MySQL db. Standardizing capitalization of MRNumber across code.
</commit_message>
<xml_diff>
--- a/Current Patients/KGID_Translation_Test.xlsx
+++ b/Current Patients/KGID_Translation_Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Perf Python Project\KetoGator\Current Patients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B54B795-3FBD-48A7-9921-95E610E08BCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86E4A06-6B2C-47CB-9127-E98852440B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="4800" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="780" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>KGID</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>KG0020</t>
+  </si>
+  <si>
+    <t>KG0002</t>
   </si>
 </sst>
 </file>
@@ -354,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,6 +392,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>